<commit_message>
Update for pandas 1.X
</commit_message>
<xml_diff>
--- a/data/output/sample_jp_data_out.xlsx
+++ b/data/output/sample_jp_data_out.xlsx
@@ -440,10 +440,10 @@
 </t>
   </si>
   <si>
-    <t>organized|time management</t>
-  </si>
-  <si>
-    <t>organizational skills|time management</t>
+    <t>time management|organized</t>
+  </si>
+  <si>
+    <t>time management|organizational skills</t>
   </si>
 </sst>
 </file>

</xml_diff>